<commit_message>
MELHOR COLETA!! Verificar se rodar no back fica mais eficiente, cancelar o contato
</commit_message>
<xml_diff>
--- a/Resultados/estabelecimentos.xlsx
+++ b/Resultados/estabelecimentos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>NOME</t>
+          <t>NOME DO ESTABELECIMENTO</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(247)</t>
+          <t>(248)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -574,7 +574,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(1.394)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -884,7 +884,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RAFAEL AUTOMÓVEIS</t>
+          <t>GARAGEM 87 MULTIMARCAS</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -894,12 +894,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>(93)</t>
+          <t>(84)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>AV. PEDRO CALAZANS, 236 - GETÚLIO VARGAS, ARACAJU - SE, 49055-520</t>
+          <t>SÃO JOSÉ, ARACAJU - SE, 49010-340</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GARAGEM 87 MULTIMARCAS</t>
+          <t>RAFAEL AUTOMÓVEIS</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -926,12 +926,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>(84)</t>
+          <t>(93)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>SÃO JOSÉ, ARACAJU - SE, 49010-340</t>
+          <t>AV. PEDRO CALAZANS, 236 - GETÚLIO VARGAS, ARACAJU - SE, 49055-520</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1748,27 +1748,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>AUTOVOX-VEICULOS</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(49)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. COELHO E CAMPOS, 738 - SANTO ANTÔNIO, ARACAJU - SE, 49060-000</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Revendedora de carros usados</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1780,27 +1780,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>PLATINUM PREMIUM CARS</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(8)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>RUA JUAREZ CARVALHO, 41 - JARDINS, ARACAJU - SE, 49025-370</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Revendedora de carros usados</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1812,27 +1812,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>RANNON AUTOMOVEIS</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(13)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. IVO DO PRADO, 1036 - SÃO JOSÉ, ARACAJU - SE, 49015-070</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Concessionária</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1844,27 +1844,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>GILVAN VEÍCULOS</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(15)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. PEDRO CALAZANS, 97 - CENTRO, ARACAJU - SE, 49010-490</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Concessionária</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1876,27 +1876,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>S7VEN CAR MULTIMARCAS LTDA</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(28)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. PEDRO CALAZANS, 594 - GETÚLIO VARGAS, ARACAJU - SE, 49055-520</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Concessionária</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1908,27 +1908,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>CAMESA AUTOMÓVEIS</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(45)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. DES. MAYNARD, Nº 915 - PEREIRA LOBO, ARACAJU - SE, 49052-335</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Revendedora de carros usados</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1940,27 +1940,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>IMPÉRIO AUTOMÓVEIS</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(21)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>RUA, AV. PEDRO CALAZANS, 123 - CENTRO, ARACAJU - SE, 49010-490</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Concessionária</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1972,7 +1972,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>PIRES AUTOMÓVEIS</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1982,17 +1982,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(30)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. CARLOS BURLAMARQUI, 684 - GETÚLIO VARGAS, ARACAJU - SE, 49055-150</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Revendedora de carros usados</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2004,7 +2004,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>CARIRA AUTOMOVEIS</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2014,17 +2014,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(23)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. COELHO E CAMPOS, 793 - 18 DO FORTE, ARACAJU - SE, 49010-720</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Revendedora de carros usados</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2036,7 +2036,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>FÁBIO TELES AUTOMÓVEIS</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2046,17 +2046,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(31)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. PEDRO CALAZANS, 43 - CENTRO, ARACAJU - SE, 49010-490</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Concessionária</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2068,27 +2068,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>RGR AUTOMOVEIS</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(27)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. SÃO PAULO, 815 - SIQUEIRA CAMPOS, ARACAJU - SE, 49075-530</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Concessionária de veículos motorizados</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2100,27 +2100,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>IDEAL MULTIMARCAS</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(34)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. DES. MAYNARD, 370 - CIRURGIA, ARACAJU - SE, 49052-210</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Concessionária de veículos motorizados</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2132,27 +2132,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>CHEVROLET CONTORNO ARACAJU</t>
+          <t>R&amp;A AUTOMOVEIS</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>(1.395)</t>
+          <t>(18)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+          <t>AV. COELHO E CAMPOS, 766 - SANTO ANTÔNIO, ARACAJU - SE, 49060-000</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Concessionária Chevrolet</t>
+          <t>Concessionária</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2164,30 +2164,638 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>BYD TERRA SANTA ARACAJU: CONCESSIONÁRIA, CARROS ELÉTRICOS, CARROS HÍBRIDOS</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>4,9</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>(328)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>AV. MINISTRO GERALDO BARRETO SOBRAL, 1740 - GRAGERU, ARACAJU - SE, 49027-255</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Concessionária</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>MAGO AUTOMÓVEIS</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>4,9</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>(14)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>AV. COELHO E CAMPOS, 783 - CENTRO, ARACAJU - SE, 49060-000</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Revendedora de carros usados</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ARABI AUTOMÓVEIS- LOJA DE CARROS SEMINOVOS, NOVOS E USADOS - COMPRA, VENDE, TROCAR, FINANCIA</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>4,2</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>(15)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>AV. CARLOS BURLAMARQUI, 637 - CENTRO, ARACAJU - SE, 49010-660</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Revendedora de carros usados</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>SAMAM FIAT RIOMAR</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>4,4</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>(328)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>AV. MARIO JORGE MENEZES VIÊIRA, 600 - COROA DO MEIO, ARACAJU - SE, 49035-660</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Concessionária</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>PEDRINHO AUTOMOVÉIS</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>4,7</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>(23)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>AV. CARLOS BURLAMARQUI, 731 - GETÚLIO VARGAS, ARACAJU - SE, 49055-150</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Concessionária</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>FOFÃO MULTIMARCAS</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>4,9</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>(14)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>AV. PEDRO CALAZANS, 300 - GETÚLIO VARGAS, ARACAJU - SE, 49055-220</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Revendedora de carros usados</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
           <t>CHEVROLET CONTORNO ARACAJU</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B61" t="inlineStr">
         <is>
           <t>4,4</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>(1.395)</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>(1.394)</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
         <is>
           <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>Concessionária Chevrolet</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>CHEVROLET CONTORNO ARACAJU</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>4,4</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>(1.394)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>AV. PRES. TANCREDO NEVES, 1550 - JARDINS, ARACAJU - SE, 49025-620</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Concessionária Chevrolet</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>PRIMECAR AUTOMÓVEIS</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>4,6</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>(12)</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>AV. COELHO E CAMPOS, 649 - CENTRO, ARACAJU - SE, 49010-720</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Revendedora de carros usados</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ADRIANO VEICULOS</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>5,0</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>(3)</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>ROD. DOS NÁUFRAGOS - ROBALO, ARACAJU - SE, 49039-000</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Revendedora de carros usados</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>SANVEL NISSAN</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>4,5</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>(637)</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>AV. PRES. TANCREDO NEVES, 640 - JARDINS, ARACAJU - SE, 49025-620</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Concessionária Nissan</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>CIMAVEL SEMINOVOS</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>4,3</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>(803)</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>AV. OVIEDO TEIXEIRA, 1001 - JARDINS, ARACAJU - SE, 49026-100</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Concessionária Ford</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>EXCLUSIVE MULTIMARCAS - CARRO DE QUALIDADE ENCONTRA AKI</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>4,8</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>(8)</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>AV. COELHO E CAMPOS, 842 - SANTO ANTÔNIO, ARACAJU - SE, 49030-000</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Agente comercial de carros</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>GT AUTOMÓVEIS ARACAJU</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>5,0</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>(11)</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>AV. CARLOS BURLAMARQUI, 716 - CENTRO, ARACAJU - SE, 49055-150</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Revendedora de carros usados</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>CLASSE A AUTOMÓVEIS</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>4,3</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>(11)</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>AV. COELHO E CAMPOS, 784 - SANTO ANTÔNIO, ARACAJU - SE, 49060-000</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Concessionária</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>MGM AUTOMÓVEIS</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>4,9</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>(13)</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>AV. PEDRO CALAZANS, 621 - CENTRO, ARACAJU - SE, 49010-490</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Revendedora de carros usados</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>UNIĀO VEÍCULOS</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>4,3</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>(6)</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>R. BASÍLIO ROCHA - GETÚLIO VARGAS, ARACAJU - SE, 49055-110</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Concessionária</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>JONATAS AUTOMOVEIS</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>4,9</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>(14)</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>AV. CARLOS BURLAMARQUI, 759 - GETÚLIO VARGAS, ARACAJU - SE, 49055-150</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Concessionária de veículos motorizados</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>MARDISA AUTOMÓVEIS MERCEDES-BENZ - ARACAJU SE</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>4,9</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>(152)</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>AV. PRES. TANCREDO NEVES, 5033 - JABOTIANA, ARACAJU - SE, 49095-000</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Concessionária Mercedes-Benz</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Contato não disponível</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>HYUNDAI HMB TERRA SANTA ARACAJU SE</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>4,9</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>(1.852)</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>AV. MINISTRO GERALDO BARRETO SOBRAL, 246 - GRAGERU, ARACAJU - SE, 49026-010</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Concessionária Hyundai</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
         <is>
           <t>Contato não disponível</t>
         </is>

</xml_diff>